<commit_message>
build bot in group
</commit_message>
<xml_diff>
--- a/src/excel/data/somasi.xlsx
+++ b/src/excel/data/somasi.xlsx
@@ -22,44 +22,44 @@
     <t>:</t>
   </si>
   <si>
-    <t>JEMMY JOHANIS SENDUK</t>
+    <t>SINTIA WOWOR</t>
   </si>
   <si>
     <t>GO LIVE</t>
   </si>
   <si>
     <t xml:space="preserve">
-                    08/08/2020  1:10PM</t>
+                    16/06/2021  4:12PM</t>
   </si>
   <si>
     <t>Agreement Number</t>
   </si>
   <si>
-    <t xml:space="preserve">06112120003162      </t>
+    <t xml:space="preserve">06111021006591      </t>
   </si>
   <si>
     <t>Birth Place/Date</t>
   </si>
   <si>
-    <t>KIAWA , 27/01/1964</t>
+    <t>AIRMADIDI , 06/09/1993</t>
   </si>
   <si>
     <t>Mailling Address</t>
   </si>
   <si>
-    <t>jemmysenduk@gmail.com</t>
+    <t>SINTIAWOWOR@GMAIL.COM</t>
   </si>
   <si>
     <t>OS Principal</t>
   </si>
   <si>
-    <t>0.00</t>
+    <t>3,033,424.75</t>
   </si>
   <si>
     <t>OS Denda</t>
   </si>
   <si>
-    <t>10,095,200.00</t>
+    <t>2,291,400.00</t>
   </si>
   <si>
     <t>ASSET VIEW</t>
@@ -68,61 +68,61 @@
     <t>Name</t>
   </si>
   <si>
-    <t>VIVI Y KANTER</t>
+    <t>FIKLY FIRGIN MANTIRI</t>
   </si>
   <si>
     <t>Address</t>
   </si>
   <si>
-    <t>DS KARONDORAN JG I KEC LANGOWAN TIMUR KAB MINAHASA</t>
+    <t>SARONGSONG I LK V KEC AIRMADIDI KAB MINAHASA UTARA</t>
   </si>
   <si>
     <t>No. Rangka</t>
   </si>
   <si>
-    <t>MHKM5EA3JGK025859</t>
+    <t>MH1KC8218HK101981</t>
   </si>
   <si>
     <t>No. Mesin</t>
   </si>
   <si>
-    <t>1NRF165380</t>
+    <t>KC82E1099191</t>
   </si>
   <si>
     <t>Year</t>
   </si>
   <si>
-    <t>2016</t>
+    <t>2017</t>
   </si>
   <si>
     <t>CC</t>
   </si>
   <si>
-    <t>1329</t>
+    <t>14916</t>
   </si>
   <si>
     <t>Color</t>
   </si>
   <si>
-    <t>PUTIH</t>
+    <t>HITAM MERAH</t>
   </si>
   <si>
     <t>License Plate</t>
   </si>
   <si>
-    <t>DB 1908 BI</t>
+    <t>DB 3114 FH</t>
   </si>
   <si>
     <t>BPKB</t>
   </si>
   <si>
-    <t>L09805768S</t>
+    <t>N01773265S</t>
   </si>
   <si>
     <t>FAKTUR</t>
   </si>
   <si>
-    <t>RAF08001EA3J2016</t>
+    <t>FHDC001030Q</t>
   </si>
   <si>
     <t>SURAT PERINGATAN</t>

</xml_diff>